<commit_message>
ui is ready upload more than one file
</commit_message>
<xml_diff>
--- a/main/xlsx/Data_Frame_WithLabels.xlsx
+++ b/main/xlsx/Data_Frame_WithLabels.xlsx
@@ -385,7 +385,7 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
         <v>0.38</v>
@@ -396,7 +396,7 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B3">
         <v>2.868</v>
@@ -407,7 +407,7 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4">
         <v>3.159</v>
@@ -418,7 +418,7 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>4.16</v>
@@ -429,7 +429,7 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B6">
         <v>6.13</v>
@@ -440,7 +440,7 @@
     </row>
     <row r="7" spans="1:3">
       <c r="A7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>9.07</v>
@@ -451,7 +451,7 @@
     </row>
     <row r="8" spans="1:3">
       <c r="A8">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B8">
         <v>10</v>
@@ -462,7 +462,7 @@
     </row>
     <row r="9" spans="1:3">
       <c r="A9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B9">
         <v>10.42</v>
@@ -473,7 +473,7 @@
     </row>
     <row r="10" spans="1:3">
       <c r="A10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B10">
         <v>10.62</v>
@@ -484,7 +484,7 @@
     </row>
     <row r="11" spans="1:3">
       <c r="A11">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B11">
         <v>10.639</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="12" spans="1:3">
       <c r="A12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B12">
         <v>10.69</v>
@@ -506,7 +506,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>10.76</v>
@@ -517,7 +517,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B14">
         <v>10.78</v>
@@ -528,7 +528,7 @@
     </row>
     <row r="15" spans="1:3">
       <c r="A15">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B15">
         <v>11.04</v>
@@ -539,7 +539,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B16">
         <v>11.53</v>
@@ -550,7 +550,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B17">
         <v>11.73</v>
@@ -561,7 +561,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B18">
         <v>12.73</v>
@@ -572,7 +572,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B19">
         <v>14.388</v>
@@ -583,7 +583,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B20">
         <v>14.718</v>
@@ -594,7 +594,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B21">
         <v>14.922</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22">
         <v>15.118</v>
@@ -616,7 +616,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B23">
         <v>17.249</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B24">
         <v>18.871</v>
@@ -638,7 +638,7 @@
     </row>
     <row r="25" spans="1:3">
       <c r="A25">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B25">
         <v>24.72</v>
@@ -649,7 +649,7 @@
     </row>
     <row r="26" spans="1:3">
       <c r="A26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B26">
         <v>44.39</v>

</xml_diff>